<commit_message>
Update 09 November 2015 - 0646
Sesuai MoM Tgl: 29 Oktober 2015, kecuali: App Presensi dan Training &
Dev
</commit_message>
<xml_diff>
--- a/contoh_excel/daftar_jemputan.xlsx
+++ b/contoh_excel/daftar_jemputan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView minimized="1" xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>